<commit_message>
Changes in registration of Donor and Patient (Fixed error)
Fixed some errors (failed to fetch from server)
</commit_message>
<xml_diff>
--- a/Life/server/data/lifelink_db.xlsx
+++ b/Life/server/data/lifelink_db.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -746,16 +746,54 @@
         <v>45975.8218484838</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>6923425d979b4e966e58ce32</v>
+      </c>
+      <c r="B11" t="str">
+        <v>web</v>
+      </c>
+      <c r="C11" t="str">
+        <v>web@gmail.com</v>
+      </c>
+      <c r="D11" t="str">
+        <v>8904534918</v>
+      </c>
+      <c r="E11" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F11" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="b">
+        <v>0</v>
+      </c>
+      <c r="K11" t="b">
+        <v>1</v>
+      </c>
+      <c r="L11" s="1">
+        <v>45984.95185159722</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L10"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L11"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1012,13 +1050,45 @@
       <c r="I8" t="str">
         <v>High</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8">
         <v>45975.89019929398</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>6923423a979b4e966e58ce2a</v>
+      </c>
+      <c r="B9" t="str">
+        <v>arc</v>
+      </c>
+      <c r="C9" t="str">
+        <v>arc@gmail.com</v>
+      </c>
+      <c r="D9" t="str">
+        <v>8904534818</v>
+      </c>
+      <c r="E9" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F9" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="J9">
+        <v>45984.95144672454</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J8"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J9"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove node_modules and cache from repo
</commit_message>
<xml_diff>
--- a/Life/server/data/lifelink_db.xlsx
+++ b/Life/server/data/lifelink_db.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -780,20 +780,324 @@
       <c r="K11" t="b">
         <v>1</v>
       </c>
-      <c r="L11" s="1">
+      <c r="L11">
         <v>45984.95185159722</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>69234632a9d7b28957d0eb0c</v>
+      </c>
+      <c r="B12" t="str">
+        <v>mno</v>
+      </c>
+      <c r="C12" t="str">
+        <v>mno@gmail.com</v>
+      </c>
+      <c r="D12" t="str">
+        <v>9481824919</v>
+      </c>
+      <c r="E12" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="b">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>45984.96320155093</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>69234680a9d7b28957d0eb11</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Me</v>
+      </c>
+      <c r="C13" t="str">
+        <v>23a43.bhavish@sjec.ac.in</v>
+      </c>
+      <c r="D13" t="str">
+        <v>8904534919</v>
+      </c>
+      <c r="E13" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F13" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>0</v>
+      </c>
+      <c r="K13" t="b">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>45984.9641012037</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>6923b7181c52f11af60577df</v>
+      </c>
+      <c r="B14" t="str">
+        <v>mailtrap</v>
+      </c>
+      <c r="C14" t="str">
+        <v>lifelink@system.com</v>
+      </c>
+      <c r="D14" t="str">
+        <v>1234456789</v>
+      </c>
+      <c r="E14" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F14" t="str">
+        <v>Mangalore</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>0</v>
+      </c>
+      <c r="K14" t="b">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>45985.297717719906</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>6923de6730064d1b9aecd2e1</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Ananya</v>
+      </c>
+      <c r="C15" t="str">
+        <v>ananyaskulai@gmail.com</v>
+      </c>
+      <c r="D15" t="str">
+        <v>6361037723</v>
+      </c>
+      <c r="E15" t="str">
+        <v>O+</v>
+      </c>
+      <c r="F15" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G15">
+        <v>74.899521</v>
+      </c>
+      <c r="H15">
+        <v>12.9103476</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="b">
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <v>45985.4141815625</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>6923e10530064d1b9aecd323</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Ananya S Kulai</v>
+      </c>
+      <c r="C16" t="str">
+        <v>ananyaskulai@gmail.com</v>
+      </c>
+      <c r="D16" t="str">
+        <v>6361037723</v>
+      </c>
+      <c r="E16" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F16" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G16">
+        <v>77.6077312</v>
+      </c>
+      <c r="H16">
+        <v>12.9728512</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="b">
+        <v>1</v>
+      </c>
+      <c r="L16">
+        <v>45985.42193297454</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>6923e2e830064d1b9aecd366</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Bhavish</v>
+      </c>
+      <c r="C17" t="str">
+        <v>bhavish@gmail.com</v>
+      </c>
+      <c r="D17" t="str">
+        <v>9986769690</v>
+      </c>
+      <c r="E17" t="str">
+        <v>B-</v>
+      </c>
+      <c r="F17" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G17">
+        <v>74.8994941</v>
+      </c>
+      <c r="H17">
+        <v>12.9103193</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <v>45985.4275340625</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>6923e4ccc81a5010397a8964</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C18" t="str">
+        <v>lifelink@system.com</v>
+      </c>
+      <c r="D18" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E18" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F18" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G18">
+        <v>77.6077312</v>
+      </c>
+      <c r="H18">
+        <v>12.9728512</v>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="b">
+        <v>0</v>
+      </c>
+      <c r="K18" t="b">
+        <v>1</v>
+      </c>
+      <c r="L18">
+        <v>45985.433130439815</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>6923f711f76d0536415e5e94</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C19" t="str">
+        <v>lifelink@gmail.com</v>
+      </c>
+      <c r="D19" t="str">
+        <v>7022157406</v>
+      </c>
+      <c r="E19" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F19" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G19">
+        <v>74.8996501</v>
+      </c>
+      <c r="H19">
+        <v>12.9103764</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <v>0</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <v>45985.48726598379</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L19"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1086,9 +1390,233 @@
         <v>45984.95144672454</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>6923d7e8e754f1d7bef87e55</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C10" t="str">
+        <v>ashwinishenoyb@gmail.com</v>
+      </c>
+      <c r="D10" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E10" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F10" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G10">
+        <v>77.6077312</v>
+      </c>
+      <c r="H10">
+        <v>12.9728512</v>
+      </c>
+      <c r="I10" t="str">
+        <v>High</v>
+      </c>
+      <c r="J10">
+        <v>45985.394934780095</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>6923dfc630064d1b9aecd306</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C11" t="str">
+        <v>ashenoyb@gmail.com</v>
+      </c>
+      <c r="D11" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E11" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F11" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G11">
+        <v>77.6077312</v>
+      </c>
+      <c r="H11">
+        <v>12.9728512</v>
+      </c>
+      <c r="I11" t="str">
+        <v>High</v>
+      </c>
+      <c r="J11">
+        <v>45985.41824520833</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>6923dfe430064d1b9aecd30f</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C12" t="str">
+        <v>ashenoyb@gmail.com</v>
+      </c>
+      <c r="D12" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E12" t="str">
+        <v>O+</v>
+      </c>
+      <c r="F12" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G12">
+        <v>77.6077312</v>
+      </c>
+      <c r="H12">
+        <v>12.9728512</v>
+      </c>
+      <c r="I12" t="str">
+        <v>High</v>
+      </c>
+      <c r="J12">
+        <v>45985.41858971065</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>6923e15630064d1b9aecd32e</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C13" t="str">
+        <v>ashenoyb@gmail.com</v>
+      </c>
+      <c r="D13" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E13" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F13" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G13">
+        <v>77.6077312</v>
+      </c>
+      <c r="H13">
+        <v>12.9728512</v>
+      </c>
+      <c r="I13" t="str">
+        <v>High</v>
+      </c>
+      <c r="J13">
+        <v>45985.422877916666</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>6923e23c30064d1b9aecd354</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C14" t="str">
+        <v>ashwinishenoyb@gmail.com</v>
+      </c>
+      <c r="D14" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E14" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F14" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G14">
+        <v>77.6077312</v>
+      </c>
+      <c r="H14">
+        <v>12.9728512</v>
+      </c>
+      <c r="I14" t="str">
+        <v>High</v>
+      </c>
+      <c r="J14">
+        <v>45985.425535104165</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>6923e5a0c81a5010397a896d</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Ananya S Kulai</v>
+      </c>
+      <c r="C15" t="str">
+        <v>ananyaskulai@gmail.com</v>
+      </c>
+      <c r="D15" t="str">
+        <v>6361037723</v>
+      </c>
+      <c r="E15" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F15" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G15">
+        <v>77.6077312</v>
+      </c>
+      <c r="H15">
+        <v>12.9728512</v>
+      </c>
+      <c r="I15" t="str">
+        <v>High</v>
+      </c>
+      <c r="J15">
+        <v>45985.43557923611</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>6923f833f76d0536415e5ea7</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C16" t="str">
+        <v>ashwinishenoyb@gmail.com</v>
+      </c>
+      <c r="D16" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E16" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F16" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G16">
+        <v>74.8996566</v>
+      </c>
+      <c r="H16">
+        <v>12.9103667</v>
+      </c>
+      <c r="I16" t="str">
+        <v>Critical</v>
+      </c>
+      <c r="J16" s="1">
+        <v>45985.49062084491</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J9"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J16"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated changes-gamification and stats
</commit_message>
<xml_diff>
--- a/Life/server/data/lifelink_db.xlsx
+++ b/Life/server/data/lifelink_db.xlsx
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1088,16 +1088,92 @@
         <v>45985.48726598379</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="str">
+        <v>69283187b147c0f70a38e0ea</v>
+      </c>
+      <c r="B20" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C20" t="str">
+        <v>ashenoyb@gmail.com</v>
+      </c>
+      <c r="D20" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E20" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F20" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G20">
+        <v>77.5483533</v>
+      </c>
+      <c r="H20">
+        <v>12.9565222</v>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <v>45988.694550451386</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="str">
+        <v>692834afb147c0f70a38e12a</v>
+      </c>
+      <c r="B21" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C21" t="str">
+        <v>shenoybashwini@gmail.com</v>
+      </c>
+      <c r="D21" t="str">
+        <v>1234567890</v>
+      </c>
+      <c r="E21" t="str">
+        <v>O+</v>
+      </c>
+      <c r="F21" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G21">
+        <v>77.5483533</v>
+      </c>
+      <c r="H21">
+        <v>12.9565222</v>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="b">
+        <v>0</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="L21" s="1">
+        <v>45988.703903194444</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:L19"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:L21"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1610,13 +1686,45 @@
       <c r="I16" t="str">
         <v>Critical</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16">
         <v>45985.49062084491</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>692831b6b147c0f70a38e0f1</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Ashwini Shenoy B</v>
+      </c>
+      <c r="C17" t="str">
+        <v>ashwinishenoyb@gmail.com</v>
+      </c>
+      <c r="D17" t="str">
+        <v>7026438371</v>
+      </c>
+      <c r="E17" t="str">
+        <v>A+</v>
+      </c>
+      <c r="F17" t="str">
+        <v>My Current Location</v>
+      </c>
+      <c r="G17">
+        <v>77.5483533</v>
+      </c>
+      <c r="H17">
+        <v>12.9565222</v>
+      </c>
+      <c r="I17" t="str">
+        <v>High</v>
+      </c>
+      <c r="J17">
+        <v>45988.695100902776</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J16"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J17"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>